<commit_message>
Loading bar works, cancel button works, other small changes
optimized plotting routes
</commit_message>
<xml_diff>
--- a/ProgramSrc/allocation_results.xlsx
+++ b/ProgramSrc/allocation_results.xlsx
@@ -529,14 +529,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>San Marcos E.C.</t>
+          <t>San Marcos Elem. Sch.</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>120.779698188389</v>
+        <v>120.778807101888</v>
       </c>
       <c r="F3" t="n">
-        <v>14.8977769256005</v>
+        <v>14.8978852342351</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -599,14 +599,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Gugo E.C.</t>
+          <t>Mun. Covered Court</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>120.754567377767</v>
+        <v>120.765260684344</v>
       </c>
       <c r="F5" t="n">
-        <v>14.9020620809296</v>
+        <v>14.9142263888355</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -634,14 +634,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Calizon Dike</t>
+          <t>San Miguel Evacuation Center</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>120.749282551866</v>
+        <v>120.743854227842</v>
       </c>
       <c r="F6" t="n">
-        <v>14.9149192538653</v>
+        <v>14.9239360863606</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -669,14 +669,14 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Gatbuca Basketball Court</t>
+          <t>Barangay Hall Bulusan</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>120.766774213649</v>
+        <v>120.742556915324</v>
       </c>
       <c r="F7" t="n">
-        <v>14.9221390531142</v>
+        <v>14.9104237817507</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -704,14 +704,14 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Meysulao Dike </t>
+          <t>Calizon Dike</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>120.738828966419</v>
+        <v>120.749282551866</v>
       </c>
       <c r="F8" t="n">
-        <v>14.9103133008009</v>
+        <v>14.9149192538653</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -739,14 +739,14 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>San Marcos Elem. Sch.</t>
+          <t>Danga Dike</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>120.778807101888</v>
+        <v>120.75016278348</v>
       </c>
       <c r="F9" t="n">
-        <v>14.8978852342351</v>
+        <v>14.9271290793079</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -774,14 +774,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Balungao E.C.</t>
+          <t>Calizon Dike</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>120.761492937455</v>
+        <v>120.749282551866</v>
       </c>
       <c r="F10" t="n">
-        <v>14.9148551401837</v>
+        <v>14.9149192538653</v>
       </c>
       <c r="G10" t="n">
         <v>6</v>
@@ -879,14 +879,14 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Calizon Dike</t>
+          <t>San Jose E.C.</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>120.749282551866</v>
+        <v>120.734404217521</v>
       </c>
       <c r="F13" t="n">
-        <v>14.9149192538653</v>
+        <v>14.8832968907295</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -949,14 +949,14 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>San Jose E.C.</t>
+          <t>Mun. Covered Court</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>120.734404217521</v>
+        <v>120.765260684344</v>
       </c>
       <c r="F15" t="n">
-        <v>14.8832968907295</v>
+        <v>14.9142263888355</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -984,14 +984,14 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Barangay Hall Bulusan</t>
+          <t>Meysulao Multipurpose/E.C.</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>120.742556915324</v>
+        <v>120.739306695061</v>
       </c>
       <c r="F16" t="n">
-        <v>14.9104237817507</v>
+        <v>14.9059685215204</v>
       </c>
       <c r="G16" t="n">
         <v>56</v>
@@ -1054,14 +1054,14 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Calumpit Sports Complex</t>
+          <t>Mun. Covered Court</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>120.767571728115</v>
+        <v>120.765260684344</v>
       </c>
       <c r="F18" t="n">
-        <v>14.9185209048724</v>
+        <v>14.9142263888355</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -1089,14 +1089,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>San Marcos E.C.</t>
+          <t>GMA Kapuso E.C.</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>120.779698188389</v>
+        <v>120.796318926682</v>
       </c>
       <c r="F19" t="n">
-        <v>14.8977769256005</v>
+        <v>14.8957602136898</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -1124,14 +1124,14 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Danga Dike</t>
+          <t>San Miguel Evacuation Center</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>120.75016278348</v>
+        <v>120.743854227842</v>
       </c>
       <c r="F20" t="n">
-        <v>14.9271290793079</v>
+        <v>14.9239360863606</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
@@ -1159,14 +1159,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Calizon Dike</t>
+          <t>San Miguel Evacuation Center</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>120.749282551866</v>
+        <v>120.743854227842</v>
       </c>
       <c r="F21" t="n">
-        <v>14.9149192538653</v>
+        <v>14.9239360863606</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -1194,14 +1194,14 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Gugo E.C.</t>
+          <t>BMLTC Multi-Purpose Bldg and EC</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>120.754567377767</v>
+        <v>120.766768211462</v>
       </c>
       <c r="F22" t="n">
-        <v>14.9020620809296</v>
+        <v>14.9185376869108</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
@@ -1229,14 +1229,14 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>San Jose E.C.</t>
+          <t>San Marcos National H.S.</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>120.734404217521</v>
+        <v>120.778052198391</v>
       </c>
       <c r="F23" t="n">
-        <v>14.8832968907295</v>
+        <v>14.8938559117996</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -1299,14 +1299,14 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>San Marcos Elem. Sch.</t>
+          <t>San Jose E.C.</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>120.778807101888</v>
+        <v>120.734404217521</v>
       </c>
       <c r="F25" t="n">
-        <v>14.8978852342351</v>
+        <v>14.8832968907295</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
@@ -1334,14 +1334,14 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Doña Damiana Elem School</t>
+          <t>NV9 Multi-Purpose</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>120.74341426756</v>
+        <v>120.765656923103</v>
       </c>
       <c r="F26" t="n">
-        <v>14.9183631788682</v>
+        <v>14.8984661105575</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
@@ -1369,14 +1369,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>NV9 Multi-Purpose</t>
+          <t>F. Mendoza Memorial Elem Sch.</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>120.765656923103</v>
+        <v>120.767878787289</v>
       </c>
       <c r="F27" t="n">
-        <v>14.8984661105575</v>
+        <v>14.9176780529243</v>
       </c>
       <c r="G27" t="n">
         <v>65</v>
@@ -1404,14 +1404,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Calumpit Sports Complex</t>
+          <t>GMA Kapuso E.C.</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>120.767571728115</v>
+        <v>120.796318926682</v>
       </c>
       <c r="F28" t="n">
-        <v>14.9185209048724</v>
+        <v>14.8957602136898</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -1439,14 +1439,14 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>F. Mendoza Memorial Elem Sch.</t>
+          <t>Balungao E.C.</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>120.767878787289</v>
+        <v>120.761492937455</v>
       </c>
       <c r="F29" t="n">
-        <v>14.9176780529243</v>
+        <v>14.9148551401837</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
added user defined path and password
</commit_message>
<xml_diff>
--- a/ProgramSrc/allocation_results.xlsx
+++ b/ProgramSrc/allocation_results.xlsx
@@ -1,37 +1,78 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="AllocationResult" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>Community Name</t>
+  </si>
+  <si>
+    <t>Shelter Assigned</t>
+  </si>
+  <si>
+    <t>Shelter Level</t>
+  </si>
+  <si>
+    <t>Balite</t>
+  </si>
+  <si>
+    <t>Balungao</t>
+  </si>
+  <si>
+    <t>Buguion</t>
+  </si>
+  <si>
+    <t>Calizon</t>
+  </si>
+  <si>
+    <t>Poblacion</t>
+  </si>
+  <si>
+    <t>F. Mendoza Memorial Elem Sch.</t>
+  </si>
+  <si>
+    <t>Gatbuca Basketball Court</t>
+  </si>
+  <si>
+    <t>San Miguel Meysulao High School</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +87,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,112 +403,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Community Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Shelter Assigned</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Shelter Level</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Balite</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>F. Mendoza Memorial Elem Sch.</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Balungao</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>F. Mendoza Memorial Elem Sch.</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Buguion</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Gatbuca Basketball Court</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Calizon</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Gatbuca Basketball Court</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Poblacion</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>San Miguel Meysulao High School</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated report details and added button
</commit_message>
<xml_diff>
--- a/ProgramSrc/allocation_results.xlsx
+++ b/ProgramSrc/allocation_results.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="AllocationResult" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Community Name</t>
   </si>
@@ -25,13 +25,10 @@
     <t>Shelter Level</t>
   </si>
   <si>
-    <t>Balite</t>
-  </si>
-  <si>
     <t>Balungao</t>
   </si>
   <si>
-    <t>Buguion</t>
+    <t>Bulusan</t>
   </si>
   <si>
     <t>Calizon</t>
@@ -40,13 +37,10 @@
     <t>Poblacion</t>
   </si>
   <si>
-    <t>F. Mendoza Memorial Elem Sch.</t>
-  </si>
-  <si>
     <t>Gatbuca Basketball Court</t>
   </si>
   <si>
-    <t>San Miguel Meysulao High School</t>
+    <t>Doña Damiana Elem School</t>
   </si>
 </sst>
 </file>
@@ -404,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,7 +420,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -448,7 +442,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -459,20 +453,9 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More report details, UI update
</commit_message>
<xml_diff>
--- a/ProgramSrc/allocation_results.xlsx
+++ b/ProgramSrc/allocation_results.xlsx
@@ -14,33 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Community Name</t>
   </si>
   <si>
+    <t>Allocated Population</t>
+  </si>
+  <si>
     <t>Shelter Assigned</t>
   </si>
   <si>
     <t>Shelter Level</t>
   </si>
   <si>
+    <t>Balite</t>
+  </si>
+  <si>
     <t>Balungao</t>
   </si>
   <si>
     <t>Bulusan</t>
   </si>
   <si>
-    <t>Calizon</t>
-  </si>
-  <si>
-    <t>Poblacion</t>
-  </si>
-  <si>
-    <t>Gatbuca Basketball Court</t>
-  </si>
-  <si>
-    <t>Doña Damiana Elem School</t>
+    <t>Frances</t>
+  </si>
+  <si>
+    <t>Gatbuca</t>
+  </si>
+  <si>
+    <t>Iba O'Este</t>
+  </si>
+  <si>
+    <t>San Miguel Meysulao High School</t>
+  </si>
+  <si>
+    <t>Frances E.C.</t>
   </si>
 </sst>
 </file>
@@ -398,13 +407,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,48 +423,91 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
+      <c r="B6">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>601</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correct calling of run_optimization
</commit_message>
<xml_diff>
--- a/ProgramSrc/allocation_results.xlsx
+++ b/ProgramSrc/allocation_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Community Name</t>
   </si>
@@ -34,48 +34,18 @@
     <t>Balungao</t>
   </si>
   <si>
-    <t>Buguion</t>
-  </si>
-  <si>
-    <t>Bulusan</t>
-  </si>
-  <si>
-    <t>Calizon</t>
-  </si>
-  <si>
     <t>Calumpang</t>
   </si>
   <si>
-    <t>Caniogan</t>
-  </si>
-  <si>
-    <t>Corazon</t>
-  </si>
-  <si>
     <t>Frances</t>
   </si>
   <si>
     <t>Gatbuca</t>
   </si>
   <si>
-    <t>Gugo</t>
-  </si>
-  <si>
-    <t>Iba Este</t>
-  </si>
-  <si>
-    <t>Iba O'Este</t>
-  </si>
-  <si>
     <t>Longos</t>
   </si>
   <si>
-    <t>Meysulao</t>
-  </si>
-  <si>
-    <t>Meyto</t>
-  </si>
-  <si>
     <t>Palimbang</t>
   </si>
   <si>
@@ -85,64 +55,28 @@
     <t>Pio Cruzcosa</t>
   </si>
   <si>
-    <t>Poblacion</t>
-  </si>
-  <si>
-    <t>Pungo</t>
-  </si>
-  <si>
     <t>San Jose</t>
   </si>
   <si>
-    <t>San Marcos</t>
-  </si>
-  <si>
-    <t>San Miguel</t>
-  </si>
-  <si>
     <t>Santa Lucia</t>
   </si>
   <si>
-    <t>Santo Niño</t>
-  </si>
-  <si>
-    <t>Sapang Bayan</t>
-  </si>
-  <si>
     <t>Sergio Bayan</t>
   </si>
   <si>
-    <t>Sucol</t>
-  </si>
-  <si>
-    <t>Brgy. Hall Sta. Lucia</t>
-  </si>
-  <si>
-    <t>MEYTO Multi-Purpose/ E.C.</t>
-  </si>
-  <si>
-    <t>Gatbuca Basketball Court</t>
-  </si>
-  <si>
-    <t>Gugo E.C.</t>
-  </si>
-  <si>
-    <t>Barangay Hall Bulusan</t>
-  </si>
-  <si>
-    <t>San Marcos National H.S.</t>
-  </si>
-  <si>
-    <t>NV9 Multi-Purpose</t>
-  </si>
-  <si>
-    <t>BMLTC Multi-Purpose Bldg and EC</t>
-  </si>
-  <si>
-    <t>San Marcos E.C.</t>
-  </si>
-  <si>
-    <t>Mun. Covered Court</t>
+    <t>Doña Damiana Elem School</t>
+  </si>
+  <si>
+    <t>Calizon Dike</t>
+  </si>
+  <si>
+    <t>Frances E.C.</t>
+  </si>
+  <si>
+    <t>GMA Kapuso E.C.</t>
+  </si>
+  <si>
+    <t>San Miguel Meysulao High School</t>
   </si>
 </sst>
 </file>
@@ -500,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -528,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -542,7 +476,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -556,7 +490,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -567,10 +501,10 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -581,10 +515,10 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -598,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -612,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -626,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -637,10 +571,10 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -651,10 +585,10 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -665,10 +599,10 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -682,247 +616,9 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>601</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>56</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20">
-        <v>92</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25">
-        <v>17</v>
-      </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28">
-        <v>65</v>
-      </c>
-      <c r="C28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30">
         <v>1</v>
       </c>
     </row>

</xml_diff>